<commit_message>
2022-06-17 Se agrega scanners y se elimina physical status
</commit_message>
<xml_diff>
--- a/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/plantilla_reporte_produccion_historial_cambios_puebla.xlsx
+++ b/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/plantilla_reporte_produccion_historial_cambios_puebla.xlsx
@@ -14,32 +14,58 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="control de cambios" sheetId="3" r:id="rId2"/>
+    <sheet name="Aux" sheetId="5" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="DATA1" localSheetId="2">#REF!</definedName>
     <definedName name="DATA1">#REF!</definedName>
+    <definedName name="DATA10" localSheetId="2">#REF!</definedName>
     <definedName name="DATA10">#REF!</definedName>
+    <definedName name="DATA11" localSheetId="2">#REF!</definedName>
     <definedName name="DATA11">#REF!</definedName>
+    <definedName name="DATA12" localSheetId="2">#REF!</definedName>
     <definedName name="DATA12">#REF!</definedName>
+    <definedName name="DATA13" localSheetId="2">#REF!</definedName>
     <definedName name="DATA13">#REF!</definedName>
+    <definedName name="DATA14" localSheetId="2">#REF!</definedName>
     <definedName name="DATA14">#REF!</definedName>
+    <definedName name="DATA15" localSheetId="2">#REF!</definedName>
     <definedName name="DATA15">#REF!</definedName>
+    <definedName name="DATA16" localSheetId="2">#REF!</definedName>
     <definedName name="DATA16">#REF!</definedName>
+    <definedName name="DATA2" localSheetId="2">#REF!</definedName>
     <definedName name="DATA2">#REF!</definedName>
+    <definedName name="DATA3" localSheetId="2">#REF!</definedName>
     <definedName name="DATA3">#REF!</definedName>
+    <definedName name="DATA4" localSheetId="2">#REF!</definedName>
     <definedName name="DATA4">#REF!</definedName>
+    <definedName name="DATA5" localSheetId="2">#REF!</definedName>
     <definedName name="DATA5">#REF!</definedName>
+    <definedName name="DATA6" localSheetId="2">#REF!</definedName>
     <definedName name="DATA6">#REF!</definedName>
+    <definedName name="DATA7" localSheetId="2">#REF!</definedName>
     <definedName name="DATA7">#REF!</definedName>
+    <definedName name="DATA8" localSheetId="2">#REF!</definedName>
     <definedName name="DATA8">#REF!</definedName>
+    <definedName name="DATA9" localSheetId="2">#REF!</definedName>
     <definedName name="DATA9">#REF!</definedName>
+    <definedName name="TEST1" localSheetId="2">#REF!</definedName>
     <definedName name="TEST1">#REF!</definedName>
+    <definedName name="TEST2" localSheetId="2">#REF!</definedName>
     <definedName name="TEST2">#REF!</definedName>
+    <definedName name="TEST3" localSheetId="2">#REF!</definedName>
     <definedName name="TEST3">#REF!</definedName>
+    <definedName name="TEST4" localSheetId="2">#REF!</definedName>
     <definedName name="TEST4">#REF!</definedName>
+    <definedName name="TEST5" localSheetId="2">#REF!</definedName>
     <definedName name="TEST5">#REF!</definedName>
+    <definedName name="TEST6" localSheetId="2">#REF!</definedName>
     <definedName name="TEST6">#REF!</definedName>
+    <definedName name="TESTHKEY" localSheetId="2">#REF!</definedName>
     <definedName name="TESTHKEY">#REF!</definedName>
+    <definedName name="TESTKEYS" localSheetId="2">#REF!</definedName>
     <definedName name="TESTKEYS">#REF!</definedName>
+    <definedName name="TESTVKEY" localSheetId="2">#REF!</definedName>
     <definedName name="TESTVKEY">#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -52,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t xml:space="preserve">Control de cambios </t>
   </si>
@@ -88,13 +114,19 @@
   </si>
   <si>
     <t>La bitácora de producción, ahora se genera a tráves del nuevo Portal de Bitácoras de Producción con la clave PRF014-04.</t>
+  </si>
+  <si>
+    <t>thyssenkrupp Materials de México S.A de C.V.</t>
+  </si>
+  <si>
+    <t>Bitácora de Producción</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,8 +154,16 @@
       <name val="TKTypeMedium"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +173,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7F7F7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -201,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -209,6 +255,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -225,6 +281,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -233,20 +298,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -533,7 +586,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
@@ -549,7 +602,7 @@
   <dimension ref="A2:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:M7"/>
+      <selection activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,218 +611,199 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6">
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10">
         <v>43685</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="11" t="s">
+      <c r="F4" s="11"/>
+      <c r="G4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6">
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10">
         <v>44139</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="11" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="14"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="11" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="14"/>
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6">
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10">
         <v>44726</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="11" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="10"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="17"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="10"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="17"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="10"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="17"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="10"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:M3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:M5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:M6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:M7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:M8"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:M11"/>
@@ -779,8 +813,64 @@
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:M10"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:M7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:M8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:M3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="203" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
2022-08-11 Se modifica agrega info platina general a reporte de producción.
</commit_message>
<xml_diff>
--- a/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/plantilla_reporte_produccion_historial_cambios_puebla.xlsx
+++ b/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/plantilla_reporte_produccion_historial_cambios_puebla.xlsx
@@ -9,63 +9,89 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
     <sheet name="control de cambios" sheetId="3" r:id="rId2"/>
     <sheet name="Aux" sheetId="5" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$CG$3</definedName>
     <definedName name="DATA1" localSheetId="2">#REF!</definedName>
+    <definedName name="DATA1" localSheetId="0">#REF!</definedName>
     <definedName name="DATA1">#REF!</definedName>
     <definedName name="DATA10" localSheetId="2">#REF!</definedName>
+    <definedName name="DATA10" localSheetId="0">#REF!</definedName>
     <definedName name="DATA10">#REF!</definedName>
     <definedName name="DATA11" localSheetId="2">#REF!</definedName>
+    <definedName name="DATA11" localSheetId="0">#REF!</definedName>
     <definedName name="DATA11">#REF!</definedName>
     <definedName name="DATA12" localSheetId="2">#REF!</definedName>
+    <definedName name="DATA12" localSheetId="0">#REF!</definedName>
     <definedName name="DATA12">#REF!</definedName>
     <definedName name="DATA13" localSheetId="2">#REF!</definedName>
+    <definedName name="DATA13" localSheetId="0">#REF!</definedName>
     <definedName name="DATA13">#REF!</definedName>
     <definedName name="DATA14" localSheetId="2">#REF!</definedName>
+    <definedName name="DATA14" localSheetId="0">#REF!</definedName>
     <definedName name="DATA14">#REF!</definedName>
     <definedName name="DATA15" localSheetId="2">#REF!</definedName>
+    <definedName name="DATA15" localSheetId="0">#REF!</definedName>
     <definedName name="DATA15">#REF!</definedName>
     <definedName name="DATA16" localSheetId="2">#REF!</definedName>
+    <definedName name="DATA16" localSheetId="0">#REF!</definedName>
     <definedName name="DATA16">#REF!</definedName>
     <definedName name="DATA2" localSheetId="2">#REF!</definedName>
+    <definedName name="DATA2" localSheetId="0">#REF!</definedName>
     <definedName name="DATA2">#REF!</definedName>
     <definedName name="DATA3" localSheetId="2">#REF!</definedName>
+    <definedName name="DATA3" localSheetId="0">#REF!</definedName>
     <definedName name="DATA3">#REF!</definedName>
     <definedName name="DATA4" localSheetId="2">#REF!</definedName>
+    <definedName name="DATA4" localSheetId="0">#REF!</definedName>
     <definedName name="DATA4">#REF!</definedName>
     <definedName name="DATA5" localSheetId="2">#REF!</definedName>
+    <definedName name="DATA5" localSheetId="0">#REF!</definedName>
     <definedName name="DATA5">#REF!</definedName>
     <definedName name="DATA6" localSheetId="2">#REF!</definedName>
+    <definedName name="DATA6" localSheetId="0">#REF!</definedName>
     <definedName name="DATA6">#REF!</definedName>
     <definedName name="DATA7" localSheetId="2">#REF!</definedName>
+    <definedName name="DATA7" localSheetId="0">#REF!</definedName>
     <definedName name="DATA7">#REF!</definedName>
     <definedName name="DATA8" localSheetId="2">#REF!</definedName>
+    <definedName name="DATA8" localSheetId="0">#REF!</definedName>
     <definedName name="DATA8">#REF!</definedName>
     <definedName name="DATA9" localSheetId="2">#REF!</definedName>
+    <definedName name="DATA9" localSheetId="0">#REF!</definedName>
     <definedName name="DATA9">#REF!</definedName>
     <definedName name="TEST1" localSheetId="2">#REF!</definedName>
+    <definedName name="TEST1" localSheetId="0">#REF!</definedName>
     <definedName name="TEST1">#REF!</definedName>
     <definedName name="TEST2" localSheetId="2">#REF!</definedName>
+    <definedName name="TEST2" localSheetId="0">#REF!</definedName>
     <definedName name="TEST2">#REF!</definedName>
     <definedName name="TEST3" localSheetId="2">#REF!</definedName>
+    <definedName name="TEST3" localSheetId="0">#REF!</definedName>
     <definedName name="TEST3">#REF!</definedName>
     <definedName name="TEST4" localSheetId="2">#REF!</definedName>
+    <definedName name="TEST4" localSheetId="0">#REF!</definedName>
     <definedName name="TEST4">#REF!</definedName>
     <definedName name="TEST5" localSheetId="2">#REF!</definedName>
+    <definedName name="TEST5" localSheetId="0">#REF!</definedName>
     <definedName name="TEST5">#REF!</definedName>
     <definedName name="TEST6" localSheetId="2">#REF!</definedName>
+    <definedName name="TEST6" localSheetId="0">#REF!</definedName>
     <definedName name="TEST6">#REF!</definedName>
     <definedName name="TESTHKEY" localSheetId="2">#REF!</definedName>
+    <definedName name="TESTHKEY" localSheetId="0">#REF!</definedName>
     <definedName name="TESTHKEY">#REF!</definedName>
     <definedName name="TESTKEYS" localSheetId="2">#REF!</definedName>
+    <definedName name="TESTKEYS" localSheetId="0">#REF!</definedName>
     <definedName name="TESTKEYS">#REF!</definedName>
     <definedName name="TESTVKEY" localSheetId="2">#REF!</definedName>
+    <definedName name="TESTVKEY" localSheetId="0">#REF!</definedName>
     <definedName name="TESTVKEY">#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -78,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="81">
   <si>
     <t xml:space="preserve">Control de cambios </t>
   </si>
@@ -120,13 +146,217 @@
   </si>
   <si>
     <t>Bitácora de Producción</t>
+  </si>
+  <si>
+    <t>09/08/2022</t>
+  </si>
+  <si>
+    <t>PRF014-04</t>
+  </si>
+  <si>
+    <t>Operador</t>
+  </si>
+  <si>
+    <t>Platina 2</t>
+  </si>
+  <si>
+    <t>Platina 1</t>
+  </si>
+  <si>
+    <t>Datos del Rollo</t>
+  </si>
+  <si>
+    <t>Lotes</t>
+  </si>
+  <si>
+    <t>Punta y Cola</t>
+  </si>
+  <si>
+    <t>Piezas de Ajuste</t>
+  </si>
+  <si>
+    <t>Balance de scrap (Platina 1)</t>
+  </si>
+  <si>
+    <t>Balance de scrap Real (Platina 1)</t>
+  </si>
+  <si>
+    <t>Balance de scrap (Platina 2)</t>
+  </si>
+  <si>
+    <t>Balance de scrap Real (Platina 2)</t>
+  </si>
+  <si>
+    <t>Balance de scrap (General)</t>
+  </si>
+  <si>
+    <t>Balance de scrap Real (General)</t>
+  </si>
+  <si>
+    <t>Planta</t>
+  </si>
+  <si>
+    <t>Linea</t>
+  </si>
+  <si>
+    <t>Supervisor</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Hora</t>
+  </si>
+  <si>
+    <t>Turno</t>
+  </si>
+  <si>
+    <t>Orden SAP</t>
+  </si>
+  <si>
+    <t>SAP Platina</t>
+  </si>
+  <si>
+    <t>Tipo de Material</t>
+  </si>
+  <si>
+    <t>Número Parte Cliente</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Orden SAP 2</t>
+  </si>
+  <si>
+    <t>SAP Platina 2</t>
+  </si>
+  <si>
+    <t>SAP Rollo</t>
+  </si>
+  <si>
+    <t>Número de Rollo</t>
+  </si>
+  <si>
+    <t>Lote de Rollo</t>
+  </si>
+  <si>
+    <t>Peso Etiqueta (kg)</t>
+  </si>
+  <si>
+    <t>Peso Regreso Rollo Real</t>
+  </si>
+  <si>
+    <t>Peso Rollo Usado</t>
+  </si>
+  <si>
+    <t>Peso Báscula</t>
+  </si>
+  <si>
+    <t>Pieza por Golpe</t>
+  </si>
+  <si>
+    <t>Órdenes por Pieza</t>
+  </si>
+  <si>
+    <t>Material Lote</t>
+  </si>
+  <si>
+    <t>No. Lote Izquierdo</t>
+  </si>
+  <si>
+    <t>No. Lote Derecho</t>
+  </si>
+  <si>
+    <t>Piezas por Paquete</t>
+  </si>
+  <si>
+    <t>Piezas (platina 1)</t>
+  </si>
+  <si>
+    <t>Piezas (platina 2)</t>
+  </si>
+  <si>
+    <t>Total Piezas</t>
+  </si>
+  <si>
+    <t>Peso de Rollo Consumido</t>
+  </si>
+  <si>
+    <t>Número de Golpes</t>
+  </si>
+  <si>
+    <t>Kg Restante de Rollo</t>
+  </si>
+  <si>
+    <t>Peso Despunte Kgs</t>
+  </si>
+  <si>
+    <t>Peso Cola Kgs</t>
+  </si>
+  <si>
+    <t>% Punta y colas</t>
+  </si>
+  <si>
+    <t>Total Piezas Ajuste</t>
+  </si>
+  <si>
+    <t>Peso Bruto Kgs</t>
+  </si>
+  <si>
+    <t>Peso Real Pieza Bruto</t>
+  </si>
+  <si>
+    <t>Peso Real Pieza Neto</t>
+  </si>
+  <si>
+    <t>Scrap Natural</t>
+  </si>
+  <si>
+    <t>Peso Neto SAP</t>
+  </si>
+  <si>
+    <t>Peso Bruto SAP</t>
+  </si>
+  <si>
+    <t>Balance de Scrap</t>
+  </si>
+  <si>
+    <t>Peso Rollo Usado Real</t>
+  </si>
+  <si>
+    <t>Peso Bruto Total Piezas Kgs</t>
+  </si>
+  <si>
+    <t>Peso Neto Total Piezas Kgs</t>
+  </si>
+  <si>
+    <t>Scrap de Ingeniería (buenas + ajuste) Total piezas</t>
+  </si>
+  <si>
+    <t>Peso Neto Total Piezas de Ajuste Kgs</t>
+  </si>
+  <si>
+    <t>Peso Punta y Colas Reales kgs</t>
+  </si>
+  <si>
+    <t>Balance de Scrap Real</t>
+  </si>
+  <si>
+    <t>comentario</t>
+  </si>
+  <si>
+    <t>General</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,8 +392,85 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,8 +489,116 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0094FF"/>
+        <bgColor rgb="FF0094FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor rgb="FF0094FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor rgb="FF0094FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor rgb="FF0094FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor rgb="FF0094FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor rgb="FF0094FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0094FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0094FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -243,11 +658,133 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD3D3D3"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -259,6 +796,162 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="20" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="21" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="22" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="21" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="22" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="21" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="22" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="21" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="22" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -301,8 +994,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="22" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="22" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="8">
+    <cellStyle name="60% - Énfasis1" xfId="5" builtinId="32"/>
+    <cellStyle name="60% - Énfasis2" xfId="6" builtinId="36"/>
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Énfasis1" xfId="4" builtinId="29"/>
+    <cellStyle name="Énfasis5" xfId="7" builtinId="45"/>
+    <cellStyle name="Entrada" xfId="3" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -582,17 +1288,553 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="0"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:CG3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="6" customWidth="1"/>
+    <col min="8" max="9" width="11.42578125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="6" customWidth="1"/>
+    <col min="12" max="13" width="14" style="6" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" style="6" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="12.28515625" style="6" customWidth="1"/>
+    <col min="19" max="19" width="19" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" style="13" customWidth="1"/>
+    <col min="21" max="24" width="12.7109375" style="14" customWidth="1"/>
+    <col min="25" max="26" width="15.28515625" style="15" customWidth="1"/>
+    <col min="27" max="33" width="11.7109375" style="13" customWidth="1"/>
+    <col min="34" max="34" width="13.140625" style="6" customWidth="1"/>
+    <col min="35" max="35" width="10.85546875" style="6" customWidth="1"/>
+    <col min="36" max="36" width="14.140625" style="6" customWidth="1"/>
+    <col min="37" max="37" width="15.140625" style="6" customWidth="1"/>
+    <col min="38" max="38" width="10.42578125" style="6" customWidth="1"/>
+    <col min="39" max="39" width="11.7109375" style="45" customWidth="1"/>
+    <col min="40" max="41" width="11.7109375" style="6" customWidth="1"/>
+    <col min="42" max="42" width="12" style="6" customWidth="1"/>
+    <col min="43" max="43" width="11.7109375" style="43" customWidth="1"/>
+    <col min="44" max="48" width="11.7109375" style="43" customWidth="1" outlineLevel="1"/>
+    <col min="49" max="49" width="11.7109375" style="45" customWidth="1" outlineLevel="1"/>
+    <col min="50" max="55" width="11.7109375" style="43" customWidth="1" outlineLevel="1"/>
+    <col min="56" max="56" width="11.7109375" style="45" customWidth="1" outlineLevel="1"/>
+    <col min="57" max="57" width="11.7109375" style="43" customWidth="1"/>
+    <col min="58" max="62" width="11.7109375" style="43" customWidth="1" outlineLevel="1"/>
+    <col min="63" max="63" width="11.7109375" style="45" customWidth="1" outlineLevel="1"/>
+    <col min="64" max="69" width="11.7109375" style="43" customWidth="1" outlineLevel="1"/>
+    <col min="70" max="70" width="11.7109375" style="45" customWidth="1" outlineLevel="1"/>
+    <col min="71" max="71" width="11.7109375" style="43" customWidth="1"/>
+    <col min="72" max="76" width="11.7109375" style="43" customWidth="1" outlineLevel="1"/>
+    <col min="77" max="77" width="11.7109375" style="45" customWidth="1" outlineLevel="1"/>
+    <col min="78" max="83" width="11.7109375" style="43" customWidth="1" outlineLevel="1"/>
+    <col min="84" max="84" width="11.7109375" style="45" customWidth="1" outlineLevel="1"/>
+    <col min="85" max="85" width="78.28515625" style="6" customWidth="1"/>
+    <col min="86" max="16384" width="9" style="37"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:85" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="44"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR1" s="38"/>
+      <c r="AS1" s="38"/>
+      <c r="AT1" s="38"/>
+      <c r="AU1" s="38"/>
+      <c r="AV1" s="38"/>
+      <c r="AW1" s="44"/>
+      <c r="AX1" s="38"/>
+      <c r="AY1" s="38"/>
+      <c r="AZ1" s="38"/>
+      <c r="BA1" s="38"/>
+      <c r="BB1" s="38"/>
+      <c r="BC1" s="38"/>
+      <c r="BD1" s="44"/>
+      <c r="BE1" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="BF1" s="38"/>
+      <c r="BG1" s="38"/>
+      <c r="BH1" s="38"/>
+      <c r="BI1" s="38"/>
+      <c r="BJ1" s="38"/>
+      <c r="BK1" s="44"/>
+      <c r="BL1" s="38"/>
+      <c r="BM1" s="38"/>
+      <c r="BN1" s="38"/>
+      <c r="BO1" s="38"/>
+      <c r="BP1" s="38"/>
+      <c r="BQ1" s="38"/>
+      <c r="BR1" s="44"/>
+      <c r="BS1" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="BT1" s="38"/>
+      <c r="BU1" s="38"/>
+      <c r="BV1" s="38"/>
+      <c r="BW1" s="38"/>
+      <c r="BX1" s="38"/>
+      <c r="BY1" s="44"/>
+      <c r="BZ1" s="38"/>
+      <c r="CA1" s="38"/>
+      <c r="CB1" s="38"/>
+      <c r="CC1" s="38"/>
+      <c r="CD1" s="38"/>
+      <c r="CE1" s="38"/>
+      <c r="CF1" s="44"/>
+      <c r="CG1" s="12"/>
+    </row>
+    <row r="2" spans="1:85" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="52"/>
+      <c r="V2" s="52"/>
+      <c r="W2" s="52"/>
+      <c r="X2" s="52"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB2" s="49"/>
+      <c r="AC2" s="49"/>
+      <c r="AD2" s="49"/>
+      <c r="AE2" s="49"/>
+      <c r="AF2" s="49"/>
+      <c r="AG2" s="49"/>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL2" s="50"/>
+      <c r="AM2" s="50"/>
+      <c r="AN2" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO2" s="50"/>
+      <c r="AP2" s="50"/>
+      <c r="AQ2" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR2" s="51"/>
+      <c r="AS2" s="51"/>
+      <c r="AT2" s="51"/>
+      <c r="AU2" s="51"/>
+      <c r="AV2" s="51"/>
+      <c r="AW2" s="51"/>
+      <c r="AX2" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="AY2" s="51"/>
+      <c r="AZ2" s="51"/>
+      <c r="BA2" s="51"/>
+      <c r="BB2" s="51"/>
+      <c r="BC2" s="51"/>
+      <c r="BD2" s="51"/>
+      <c r="BE2" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="BF2" s="47"/>
+      <c r="BG2" s="47"/>
+      <c r="BH2" s="47"/>
+      <c r="BI2" s="47"/>
+      <c r="BJ2" s="47"/>
+      <c r="BK2" s="47"/>
+      <c r="BL2" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="BM2" s="47"/>
+      <c r="BN2" s="47"/>
+      <c r="BO2" s="47"/>
+      <c r="BP2" s="47"/>
+      <c r="BQ2" s="47"/>
+      <c r="BR2" s="47"/>
+      <c r="BS2" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="BT2" s="48"/>
+      <c r="BU2" s="48"/>
+      <c r="BV2" s="48"/>
+      <c r="BW2" s="48"/>
+      <c r="BX2" s="48"/>
+      <c r="BY2" s="48"/>
+      <c r="BZ2" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="CA2" s="48"/>
+      <c r="CB2" s="48"/>
+      <c r="CC2" s="48"/>
+      <c r="CD2" s="48"/>
+      <c r="CE2" s="48"/>
+      <c r="CF2" s="48"/>
+      <c r="CG2" s="12"/>
+    </row>
+    <row r="3" spans="1:85" s="36" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="U3" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="V3" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="W3" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="X3" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y3" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z3" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA3" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB3" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC3" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD3" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE3" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF3" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG3" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH3" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI3" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ3" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK3" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL3" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM3" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN3" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO3" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP3" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="AQ3" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR3" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS3" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT3" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="AU3" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="AV3" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW3" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX3" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="AY3" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ3" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="BA3" s="71" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB3" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC3" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="BD3" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="BE3" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="BF3" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="BG3" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH3" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="BI3" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="BJ3" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="BK3" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="BL3" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="BM3" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="BN3" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="BO3" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="BP3" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="BQ3" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="BR3" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="BS3" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="BT3" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="BU3" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="BV3" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="BW3" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="BX3" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="BY3" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="BZ3" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="CA3" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="CB3" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="CC3" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="CD3" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="CE3" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="CF3" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="CG3" s="35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A3:CG3"/>
+  <mergeCells count="15">
+    <mergeCell ref="R2:X2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="BL2:BR2"/>
+    <mergeCell ref="BS2:BY2"/>
+    <mergeCell ref="BZ2:CF2"/>
+    <mergeCell ref="AA2:AG2"/>
+    <mergeCell ref="AK2:AM2"/>
+    <mergeCell ref="AN2:AP2"/>
+    <mergeCell ref="AQ2:AW2"/>
+    <mergeCell ref="AX2:BD2"/>
+    <mergeCell ref="BE2:BK2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -601,8 +1843,8 @@
   <sheetPr codeName="Hoja8"/>
   <dimension ref="A2:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M23" sqref="M22:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,196 +1853,196 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6" t="s">
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6" t="s">
+      <c r="F3" s="58"/>
+      <c r="G3" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10">
+      <c r="C4" s="60"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="62">
         <v>43685</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12" t="s">
+      <c r="F4" s="63"/>
+      <c r="G4" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="14"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="66"/>
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10">
+      <c r="C5" s="60"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="62">
         <v>44139</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12" t="s">
+      <c r="F5" s="63"/>
+      <c r="G5" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="14"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="66"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10" t="s">
+      <c r="C6" s="60"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12" t="s">
+      <c r="F6" s="63"/>
+      <c r="G6" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="14"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="66"/>
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10">
+      <c r="C7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="62">
         <v>44726</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12" t="s">
+      <c r="F7" s="63"/>
+      <c r="G7" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="66"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="17"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="69"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="17"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="68"/>
+      <c r="L9" s="68"/>
+      <c r="M9" s="69"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="17"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="69"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="17"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="68"/>
+      <c r="M11" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="28">
@@ -850,15 +2092,15 @@
   <sheetData>
     <row r="1" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18" t="s">
+      <c r="C1" s="70"/>
+      <c r="D1" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
       <c r="G1" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
2022-08-22 Se realizan correcciones al Sistema de Bitácoras.
</commit_message>
<xml_diff>
--- a/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/plantilla_reporte_produccion_historial_cambios_puebla.xlsx
+++ b/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/plantilla_reporte_produccion_historial_cambios_puebla.xlsx
@@ -784,7 +784,7 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -922,35 +922,74 @@
     <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="22" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="22" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -958,47 +997,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="22" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="22" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1290,11 +1293,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:CG3"/>
+  <dimension ref="A1:CG7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1346,18 +1349,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:85" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="56" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
       <c r="I1" s="46"/>
       <c r="J1" s="46" t="s">
         <v>15</v>
@@ -1445,116 +1448,116 @@
       <c r="CG1" s="12"/>
     </row>
     <row r="2" spans="1:85" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="7"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="52" t="s">
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="52"/>
-      <c r="W2" s="52"/>
-      <c r="X2" s="52"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
       <c r="Y2" s="16"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="49" t="s">
+      <c r="AA2" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="AB2" s="49"/>
-      <c r="AC2" s="49"/>
-      <c r="AD2" s="49"/>
-      <c r="AE2" s="49"/>
-      <c r="AF2" s="49"/>
-      <c r="AG2" s="49"/>
+      <c r="AB2" s="51"/>
+      <c r="AC2" s="51"/>
+      <c r="AD2" s="51"/>
+      <c r="AE2" s="51"/>
+      <c r="AF2" s="51"/>
+      <c r="AG2" s="51"/>
       <c r="AH2" s="12"/>
       <c r="AI2" s="12"/>
       <c r="AJ2" s="12"/>
-      <c r="AK2" s="50" t="s">
+      <c r="AK2" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="AL2" s="50"/>
-      <c r="AM2" s="50"/>
-      <c r="AN2" s="50" t="s">
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="AO2" s="50"/>
-      <c r="AP2" s="50"/>
-      <c r="AQ2" s="51" t="s">
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="57"/>
+      <c r="AQ2" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="AR2" s="51"/>
-      <c r="AS2" s="51"/>
-      <c r="AT2" s="51"/>
-      <c r="AU2" s="51"/>
-      <c r="AV2" s="51"/>
-      <c r="AW2" s="51"/>
-      <c r="AX2" s="51" t="s">
+      <c r="AR2" s="58"/>
+      <c r="AS2" s="58"/>
+      <c r="AT2" s="58"/>
+      <c r="AU2" s="58"/>
+      <c r="AV2" s="58"/>
+      <c r="AW2" s="58"/>
+      <c r="AX2" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="AY2" s="51"/>
-      <c r="AZ2" s="51"/>
-      <c r="BA2" s="51"/>
-      <c r="BB2" s="51"/>
-      <c r="BC2" s="51"/>
-      <c r="BD2" s="51"/>
-      <c r="BE2" s="47" t="s">
+      <c r="AY2" s="58"/>
+      <c r="AZ2" s="58"/>
+      <c r="BA2" s="58"/>
+      <c r="BB2" s="58"/>
+      <c r="BC2" s="58"/>
+      <c r="BD2" s="58"/>
+      <c r="BE2" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="BF2" s="47"/>
-      <c r="BG2" s="47"/>
-      <c r="BH2" s="47"/>
-      <c r="BI2" s="47"/>
-      <c r="BJ2" s="47"/>
-      <c r="BK2" s="47"/>
-      <c r="BL2" s="47" t="s">
+      <c r="BF2" s="55"/>
+      <c r="BG2" s="55"/>
+      <c r="BH2" s="55"/>
+      <c r="BI2" s="55"/>
+      <c r="BJ2" s="55"/>
+      <c r="BK2" s="55"/>
+      <c r="BL2" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="BM2" s="47"/>
-      <c r="BN2" s="47"/>
-      <c r="BO2" s="47"/>
-      <c r="BP2" s="47"/>
-      <c r="BQ2" s="47"/>
-      <c r="BR2" s="47"/>
-      <c r="BS2" s="48" t="s">
+      <c r="BM2" s="55"/>
+      <c r="BN2" s="55"/>
+      <c r="BO2" s="55"/>
+      <c r="BP2" s="55"/>
+      <c r="BQ2" s="55"/>
+      <c r="BR2" s="55"/>
+      <c r="BS2" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="BT2" s="48"/>
-      <c r="BU2" s="48"/>
-      <c r="BV2" s="48"/>
-      <c r="BW2" s="48"/>
-      <c r="BX2" s="48"/>
-      <c r="BY2" s="48"/>
-      <c r="BZ2" s="48" t="s">
+      <c r="BT2" s="56"/>
+      <c r="BU2" s="56"/>
+      <c r="BV2" s="56"/>
+      <c r="BW2" s="56"/>
+      <c r="BX2" s="56"/>
+      <c r="BY2" s="56"/>
+      <c r="BZ2" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="CA2" s="48"/>
-      <c r="CB2" s="48"/>
-      <c r="CC2" s="48"/>
-      <c r="CD2" s="48"/>
-      <c r="CE2" s="48"/>
-      <c r="CF2" s="48"/>
+      <c r="CA2" s="56"/>
+      <c r="CB2" s="56"/>
+      <c r="CC2" s="56"/>
+      <c r="CD2" s="56"/>
+      <c r="CE2" s="56"/>
+      <c r="CF2" s="56"/>
       <c r="CG2" s="12"/>
     </row>
     <row r="3" spans="1:85" s="36" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1714,7 +1717,7 @@
       <c r="AZ3" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="BA3" s="71" t="s">
+      <c r="BA3" s="47" t="s">
         <v>75</v>
       </c>
       <c r="BB3" s="40" t="s">
@@ -1756,7 +1759,7 @@
       <c r="BN3" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="BO3" s="72" t="s">
+      <c r="BO3" s="48" t="s">
         <v>75</v>
       </c>
       <c r="BP3" s="42" t="s">
@@ -1798,7 +1801,7 @@
       <c r="CB3" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="CC3" s="72" t="s">
+      <c r="CC3" s="48" t="s">
         <v>75</v>
       </c>
       <c r="CD3" s="42" t="s">
@@ -1813,16 +1816,13 @@
       <c r="CG3" s="35" t="s">
         <v>79</v>
       </c>
+    </row>
+    <row r="7" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="C7" s="73"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:CG3"/>
   <mergeCells count="15">
-    <mergeCell ref="R2:X2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="C1:H1"/>
     <mergeCell ref="BL2:BR2"/>
     <mergeCell ref="BS2:BY2"/>
     <mergeCell ref="BZ2:CF2"/>
@@ -1832,6 +1832,12 @@
     <mergeCell ref="AQ2:AW2"/>
     <mergeCell ref="AX2:BD2"/>
     <mergeCell ref="BE2:BK2"/>
+    <mergeCell ref="R2:X2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="C1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1853,44 +1859,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58" t="s">
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58" t="s">
+      <c r="F3" s="71"/>
+      <c r="G3" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -1905,15 +1911,15 @@
         <v>43685</v>
       </c>
       <c r="F4" s="63"/>
-      <c r="G4" s="64" t="s">
+      <c r="G4" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="66"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="69"/>
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -1928,15 +1934,15 @@
         <v>44139</v>
       </c>
       <c r="F5" s="63"/>
-      <c r="G5" s="64" t="s">
+      <c r="G5" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="66"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="69"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -1951,15 +1957,15 @@
         <v>9</v>
       </c>
       <c r="F6" s="63"/>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="66"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="69"/>
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -1974,15 +1980,15 @@
         <v>44726</v>
       </c>
       <c r="F7" s="63"/>
-      <c r="G7" s="64" t="s">
+      <c r="G7" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="66"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="69"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -1991,13 +1997,13 @@
       <c r="D8" s="61"/>
       <c r="E8" s="62"/>
       <c r="F8" s="63"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="68"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="68"/>
-      <c r="M8" s="69"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="66"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -2006,13 +2012,13 @@
       <c r="D9" s="61"/>
       <c r="E9" s="62"/>
       <c r="F9" s="63"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="68"/>
-      <c r="K9" s="68"/>
-      <c r="L9" s="68"/>
-      <c r="M9" s="69"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="66"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -2021,13 +2027,13 @@
       <c r="D10" s="61"/>
       <c r="E10" s="62"/>
       <c r="F10" s="63"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="68"/>
-      <c r="K10" s="68"/>
-      <c r="L10" s="68"/>
-      <c r="M10" s="69"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="66"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -2036,16 +2042,35 @@
       <c r="D11" s="61"/>
       <c r="E11" s="62"/>
       <c r="F11" s="63"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="68"/>
-      <c r="I11" s="68"/>
-      <c r="J11" s="68"/>
-      <c r="K11" s="68"/>
-      <c r="L11" s="68"/>
-      <c r="M11" s="69"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:M3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:M7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:M8"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:M11"/>
@@ -2055,25 +2080,6 @@
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:M10"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:M7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:M8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:M5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:M6"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:M3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="203" r:id="rId1"/>
@@ -2092,15 +2098,15 @@
   <sheetData>
     <row r="1" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70" t="s">
+      <c r="C1" s="72"/>
+      <c r="D1" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
       <c r="G1" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
2023-08-10 Se agrega cliente a reporte de produccion.
</commit_message>
<xml_diff>
--- a/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/plantilla_reporte_produccion_historial_cambios_puebla.xlsx
+++ b/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/plantilla_reporte_produccion_historial_cambios_puebla.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\NuevoPortal\CódigoFuente\BitacorasProduccion\Content\plantillas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3355BC-40F8-4AB7-B5A6-184B068AEF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Aux" sheetId="5" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$CG$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$CH$3</definedName>
     <definedName name="DATA1" localSheetId="2">#REF!</definedName>
     <definedName name="DATA1" localSheetId="0">#REF!</definedName>
     <definedName name="DATA1">#REF!</definedName>
@@ -104,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="82">
   <si>
     <t xml:space="preserve">Control de cambios </t>
   </si>
@@ -347,12 +348,15 @@
   </si>
   <si>
     <t>General</t>
+  </si>
+  <si>
+    <t>Cliente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -784,7 +788,7 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -829,9 +833,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -928,15 +929,33 @@
     <xf numFmtId="164" fontId="15" fillId="22" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -946,17 +965,11 @@
     <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -974,15 +987,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -991,17 +995,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1289,15 +1296,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:CG7"/>
+  <dimension ref="A1:CH7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1315,73 +1322,75 @@
     <col min="12" max="13" width="14" style="6" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" style="6" customWidth="1"/>
     <col min="15" max="15" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="12.28515625" style="6" customWidth="1"/>
-    <col min="19" max="19" width="19" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" style="13" customWidth="1"/>
-    <col min="21" max="24" width="12.7109375" style="14" customWidth="1"/>
-    <col min="25" max="26" width="15.28515625" style="15" customWidth="1"/>
-    <col min="27" max="33" width="11.7109375" style="13" customWidth="1"/>
-    <col min="34" max="34" width="13.140625" style="6" customWidth="1"/>
-    <col min="35" max="35" width="10.85546875" style="6" customWidth="1"/>
-    <col min="36" max="36" width="14.140625" style="6" customWidth="1"/>
-    <col min="37" max="37" width="15.140625" style="6" customWidth="1"/>
-    <col min="38" max="38" width="10.42578125" style="6" customWidth="1"/>
-    <col min="39" max="39" width="11.7109375" style="45" customWidth="1"/>
-    <col min="40" max="41" width="11.7109375" style="6" customWidth="1"/>
-    <col min="42" max="42" width="12" style="6" customWidth="1"/>
-    <col min="43" max="43" width="11.7109375" style="43" customWidth="1"/>
-    <col min="44" max="48" width="11.7109375" style="43" customWidth="1" outlineLevel="1"/>
-    <col min="49" max="49" width="11.7109375" style="45" customWidth="1" outlineLevel="1"/>
-    <col min="50" max="55" width="11.7109375" style="43" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="11.7109375" style="45" customWidth="1" outlineLevel="1"/>
-    <col min="57" max="57" width="11.7109375" style="43" customWidth="1"/>
-    <col min="58" max="62" width="11.7109375" style="43" customWidth="1" outlineLevel="1"/>
-    <col min="63" max="63" width="11.7109375" style="45" customWidth="1" outlineLevel="1"/>
-    <col min="64" max="69" width="11.7109375" style="43" customWidth="1" outlineLevel="1"/>
-    <col min="70" max="70" width="11.7109375" style="45" customWidth="1" outlineLevel="1"/>
-    <col min="71" max="71" width="11.7109375" style="43" customWidth="1"/>
-    <col min="72" max="76" width="11.7109375" style="43" customWidth="1" outlineLevel="1"/>
-    <col min="77" max="77" width="11.7109375" style="45" customWidth="1" outlineLevel="1"/>
-    <col min="78" max="83" width="11.7109375" style="43" customWidth="1" outlineLevel="1"/>
-    <col min="84" max="84" width="11.7109375" style="45" customWidth="1" outlineLevel="1"/>
-    <col min="85" max="85" width="78.28515625" style="6" customWidth="1"/>
-    <col min="86" max="16384" width="9" style="37"/>
+    <col min="16" max="17" width="12.28515625" style="6" customWidth="1"/>
+    <col min="18" max="18" width="33.140625" style="6" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="6" customWidth="1"/>
+    <col min="20" max="20" width="19" style="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" style="13" customWidth="1"/>
+    <col min="22" max="25" width="12.7109375" style="14" customWidth="1"/>
+    <col min="26" max="27" width="15.28515625" style="15" customWidth="1"/>
+    <col min="28" max="34" width="11.7109375" style="13" customWidth="1"/>
+    <col min="35" max="35" width="13.140625" style="6" customWidth="1"/>
+    <col min="36" max="36" width="10.85546875" style="6" customWidth="1"/>
+    <col min="37" max="37" width="14.140625" style="6" customWidth="1"/>
+    <col min="38" max="38" width="15.140625" style="6" customWidth="1"/>
+    <col min="39" max="39" width="10.42578125" style="6" customWidth="1"/>
+    <col min="40" max="40" width="11.7109375" style="44" customWidth="1"/>
+    <col min="41" max="42" width="11.7109375" style="6" customWidth="1"/>
+    <col min="43" max="43" width="12" style="6" customWidth="1"/>
+    <col min="44" max="44" width="11.7109375" style="42" customWidth="1"/>
+    <col min="45" max="49" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="50" max="50" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="51" max="56" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="57" max="57" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="58" max="58" width="11.7109375" style="42" customWidth="1"/>
+    <col min="59" max="63" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="64" max="64" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="65" max="70" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="71" max="71" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="72" max="72" width="11.7109375" style="42" customWidth="1"/>
+    <col min="73" max="77" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="78" max="78" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="79" max="84" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="85" max="85" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="86" max="86" width="78.28515625" style="6" customWidth="1"/>
+    <col min="87" max="16384" width="9" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:86" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="54" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46" t="s">
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
       <c r="O1" s="12"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
       <c r="S1" s="12"/>
       <c r="T1" s="12"/>
-      <c r="U1" s="9"/>
+      <c r="U1" s="12"/>
       <c r="V1" s="9"/>
       <c r="W1" s="9"/>
       <c r="X1" s="9"/>
-      <c r="Y1" s="10"/>
+      <c r="Y1" s="9"/>
       <c r="Z1" s="10"/>
-      <c r="AA1" s="12"/>
+      <c r="AA1" s="10"/>
       <c r="AB1" s="12"/>
       <c r="AC1" s="12"/>
       <c r="AD1" s="12"/>
@@ -1393,451 +1402,458 @@
       <c r="AJ1" s="12"/>
       <c r="AK1" s="12"/>
       <c r="AL1" s="12"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="43"/>
       <c r="AO1" s="12"/>
       <c r="AP1" s="12"/>
-      <c r="AQ1" s="38" t="s">
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="AR1" s="38"/>
-      <c r="AS1" s="38"/>
-      <c r="AT1" s="38"/>
-      <c r="AU1" s="38"/>
-      <c r="AV1" s="38"/>
-      <c r="AW1" s="44"/>
-      <c r="AX1" s="38"/>
-      <c r="AY1" s="38"/>
-      <c r="AZ1" s="38"/>
-      <c r="BA1" s="38"/>
-      <c r="BB1" s="38"/>
-      <c r="BC1" s="38"/>
-      <c r="BD1" s="44"/>
-      <c r="BE1" s="38" t="s">
+      <c r="AS1" s="37"/>
+      <c r="AT1" s="37"/>
+      <c r="AU1" s="37"/>
+      <c r="AV1" s="37"/>
+      <c r="AW1" s="37"/>
+      <c r="AX1" s="43"/>
+      <c r="AY1" s="37"/>
+      <c r="AZ1" s="37"/>
+      <c r="BA1" s="37"/>
+      <c r="BB1" s="37"/>
+      <c r="BC1" s="37"/>
+      <c r="BD1" s="37"/>
+      <c r="BE1" s="43"/>
+      <c r="BF1" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="BF1" s="38"/>
-      <c r="BG1" s="38"/>
-      <c r="BH1" s="38"/>
-      <c r="BI1" s="38"/>
-      <c r="BJ1" s="38"/>
-      <c r="BK1" s="44"/>
-      <c r="BL1" s="38"/>
-      <c r="BM1" s="38"/>
-      <c r="BN1" s="38"/>
-      <c r="BO1" s="38"/>
-      <c r="BP1" s="38"/>
-      <c r="BQ1" s="38"/>
-      <c r="BR1" s="44"/>
-      <c r="BS1" s="38" t="s">
+      <c r="BG1" s="37"/>
+      <c r="BH1" s="37"/>
+      <c r="BI1" s="37"/>
+      <c r="BJ1" s="37"/>
+      <c r="BK1" s="37"/>
+      <c r="BL1" s="43"/>
+      <c r="BM1" s="37"/>
+      <c r="BN1" s="37"/>
+      <c r="BO1" s="37"/>
+      <c r="BP1" s="37"/>
+      <c r="BQ1" s="37"/>
+      <c r="BR1" s="37"/>
+      <c r="BS1" s="43"/>
+      <c r="BT1" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="BT1" s="38"/>
-      <c r="BU1" s="38"/>
-      <c r="BV1" s="38"/>
-      <c r="BW1" s="38"/>
-      <c r="BX1" s="38"/>
-      <c r="BY1" s="44"/>
-      <c r="BZ1" s="38"/>
-      <c r="CA1" s="38"/>
-      <c r="CB1" s="38"/>
-      <c r="CC1" s="38"/>
-      <c r="CD1" s="38"/>
-      <c r="CE1" s="38"/>
-      <c r="CF1" s="44"/>
-      <c r="CG1" s="12"/>
+      <c r="BU1" s="37"/>
+      <c r="BV1" s="37"/>
+      <c r="BW1" s="37"/>
+      <c r="BX1" s="37"/>
+      <c r="BY1" s="37"/>
+      <c r="BZ1" s="43"/>
+      <c r="CA1" s="37"/>
+      <c r="CB1" s="37"/>
+      <c r="CC1" s="37"/>
+      <c r="CD1" s="37"/>
+      <c r="CE1" s="37"/>
+      <c r="CF1" s="37"/>
+      <c r="CG1" s="43"/>
+      <c r="CH1" s="12"/>
     </row>
-    <row r="2" spans="1:85" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+    <row r="2" spans="1:86" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
       <c r="E2" s="7"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="53" t="s">
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="49" t="s">
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="S2" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="51" t="s">
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
+      <c r="W2" s="55"/>
+      <c r="X2" s="55"/>
+      <c r="Y2" s="55"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
-      <c r="AF2" s="51"/>
-      <c r="AG2" s="51"/>
-      <c r="AH2" s="12"/>
+      <c r="AC2" s="52"/>
+      <c r="AD2" s="52"/>
+      <c r="AE2" s="52"/>
+      <c r="AF2" s="52"/>
+      <c r="AG2" s="52"/>
+      <c r="AH2" s="52"/>
       <c r="AI2" s="12"/>
       <c r="AJ2" s="12"/>
-      <c r="AK2" s="57" t="s">
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="AL2" s="57"/>
-      <c r="AM2" s="57"/>
-      <c r="AN2" s="57" t="s">
+      <c r="AM2" s="53"/>
+      <c r="AN2" s="53"/>
+      <c r="AO2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="AO2" s="57"/>
-      <c r="AP2" s="57"/>
-      <c r="AQ2" s="58" t="s">
+      <c r="AP2" s="53"/>
+      <c r="AQ2" s="53"/>
+      <c r="AR2" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="AR2" s="58"/>
-      <c r="AS2" s="58"/>
-      <c r="AT2" s="58"/>
-      <c r="AU2" s="58"/>
-      <c r="AV2" s="58"/>
-      <c r="AW2" s="58"/>
-      <c r="AX2" s="58" t="s">
+      <c r="AS2" s="54"/>
+      <c r="AT2" s="54"/>
+      <c r="AU2" s="54"/>
+      <c r="AV2" s="54"/>
+      <c r="AW2" s="54"/>
+      <c r="AX2" s="54"/>
+      <c r="AY2" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="AY2" s="58"/>
-      <c r="AZ2" s="58"/>
-      <c r="BA2" s="58"/>
-      <c r="BB2" s="58"/>
-      <c r="BC2" s="58"/>
-      <c r="BD2" s="58"/>
-      <c r="BE2" s="55" t="s">
+      <c r="AZ2" s="54"/>
+      <c r="BA2" s="54"/>
+      <c r="BB2" s="54"/>
+      <c r="BC2" s="54"/>
+      <c r="BD2" s="54"/>
+      <c r="BE2" s="54"/>
+      <c r="BF2" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="BF2" s="55"/>
-      <c r="BG2" s="55"/>
-      <c r="BH2" s="55"/>
-      <c r="BI2" s="55"/>
-      <c r="BJ2" s="55"/>
-      <c r="BK2" s="55"/>
-      <c r="BL2" s="55" t="s">
+      <c r="BG2" s="50"/>
+      <c r="BH2" s="50"/>
+      <c r="BI2" s="50"/>
+      <c r="BJ2" s="50"/>
+      <c r="BK2" s="50"/>
+      <c r="BL2" s="50"/>
+      <c r="BM2" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="BM2" s="55"/>
-      <c r="BN2" s="55"/>
-      <c r="BO2" s="55"/>
-      <c r="BP2" s="55"/>
-      <c r="BQ2" s="55"/>
-      <c r="BR2" s="55"/>
-      <c r="BS2" s="56" t="s">
+      <c r="BN2" s="50"/>
+      <c r="BO2" s="50"/>
+      <c r="BP2" s="50"/>
+      <c r="BQ2" s="50"/>
+      <c r="BR2" s="50"/>
+      <c r="BS2" s="50"/>
+      <c r="BT2" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="BT2" s="56"/>
-      <c r="BU2" s="56"/>
-      <c r="BV2" s="56"/>
-      <c r="BW2" s="56"/>
-      <c r="BX2" s="56"/>
-      <c r="BY2" s="56"/>
-      <c r="BZ2" s="56" t="s">
+      <c r="BU2" s="51"/>
+      <c r="BV2" s="51"/>
+      <c r="BW2" s="51"/>
+      <c r="BX2" s="51"/>
+      <c r="BY2" s="51"/>
+      <c r="BZ2" s="51"/>
+      <c r="CA2" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="CA2" s="56"/>
-      <c r="CB2" s="56"/>
-      <c r="CC2" s="56"/>
-      <c r="CD2" s="56"/>
-      <c r="CE2" s="56"/>
-      <c r="CF2" s="56"/>
-      <c r="CG2" s="12"/>
+      <c r="CB2" s="51"/>
+      <c r="CC2" s="51"/>
+      <c r="CD2" s="51"/>
+      <c r="CE2" s="51"/>
+      <c r="CF2" s="51"/>
+      <c r="CG2" s="51"/>
+      <c r="CH2" s="12"/>
     </row>
-    <row r="3" spans="1:85" s="36" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:86" s="35" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="20" t="s">
+      <c r="O3" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="P3" s="20" t="s">
+      <c r="P3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="20" t="s">
+      <c r="Q3" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="R3" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="S3" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="S3" s="21" t="s">
+      <c r="T3" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="T3" s="21" t="s">
+      <c r="U3" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="U3" s="22" t="s">
+      <c r="V3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="V3" s="22" t="s">
+      <c r="W3" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="W3" s="22" t="s">
+      <c r="X3" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="X3" s="22" t="s">
+      <c r="Y3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="Y3" s="23" t="s">
+      <c r="Z3" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="Z3" s="24" t="s">
+      <c r="AA3" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="AA3" s="25" t="s">
+      <c r="AB3" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="AB3" s="26" t="s">
+      <c r="AC3" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="AC3" s="26" t="s">
+      <c r="AD3" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="AD3" s="26" t="s">
+      <c r="AE3" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="AE3" s="27" t="s">
+      <c r="AF3" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AF3" s="27" t="s">
+      <c r="AG3" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="AG3" s="28" t="s">
+      <c r="AH3" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="AH3" s="17" t="s">
+      <c r="AI3" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="AI3" s="17" t="s">
+      <c r="AJ3" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="AJ3" s="17" t="s">
+      <c r="AK3" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="AK3" s="17" t="s">
+      <c r="AL3" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="AL3" s="17" t="s">
+      <c r="AM3" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="AM3" s="29" t="s">
+      <c r="AN3" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="AN3" s="30" t="s">
+      <c r="AO3" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="AO3" s="30" t="s">
+      <c r="AP3" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="AP3" s="17" t="s">
+      <c r="AQ3" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="AQ3" s="39" t="s">
+      <c r="AR3" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="AR3" s="39" t="s">
+      <c r="AS3" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="AS3" s="39" t="s">
+      <c r="AT3" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="AT3" s="39" t="s">
+      <c r="AU3" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="AU3" s="39" t="s">
+      <c r="AV3" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="AV3" s="39" t="s">
+      <c r="AW3" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="AW3" s="31" t="s">
+      <c r="AX3" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="AX3" s="40" t="s">
+      <c r="AY3" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="AY3" s="40" t="s">
+      <c r="AZ3" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="AZ3" s="40" t="s">
+      <c r="BA3" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="BA3" s="47" t="s">
+      <c r="BB3" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="BB3" s="40" t="s">
+      <c r="BC3" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="BC3" s="40" t="s">
+      <c r="BD3" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="BD3" s="32" t="s">
+      <c r="BE3" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="BE3" s="41" t="s">
+      <c r="BF3" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="BF3" s="41" t="s">
+      <c r="BG3" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="BG3" s="41" t="s">
+      <c r="BH3" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="BH3" s="41" t="s">
+      <c r="BI3" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="BI3" s="41" t="s">
+      <c r="BJ3" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="BJ3" s="41" t="s">
+      <c r="BK3" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="BK3" s="33" t="s">
+      <c r="BL3" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="BL3" s="42" t="s">
+      <c r="BM3" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="BM3" s="42" t="s">
+      <c r="BN3" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="BN3" s="42" t="s">
+      <c r="BO3" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="BO3" s="48" t="s">
+      <c r="BP3" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="BP3" s="42" t="s">
+      <c r="BQ3" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="BQ3" s="42" t="s">
+      <c r="BR3" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="BR3" s="34" t="s">
+      <c r="BS3" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="BS3" s="41" t="s">
+      <c r="BT3" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="BT3" s="41" t="s">
+      <c r="BU3" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="BU3" s="41" t="s">
+      <c r="BV3" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="BV3" s="41" t="s">
+      <c r="BW3" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="BW3" s="41" t="s">
+      <c r="BX3" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="BX3" s="41" t="s">
+      <c r="BY3" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="BY3" s="33" t="s">
+      <c r="BZ3" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="BZ3" s="42" t="s">
+      <c r="CA3" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="CA3" s="42" t="s">
+      <c r="CB3" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="CB3" s="42" t="s">
+      <c r="CC3" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="CC3" s="48" t="s">
+      <c r="CD3" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="CD3" s="42" t="s">
+      <c r="CE3" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="CE3" s="42" t="s">
+      <c r="CF3" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="CF3" s="34" t="s">
+      <c r="CG3" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="CG3" s="35" t="s">
+      <c r="CH3" s="34" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="C7" s="73"/>
+    <row r="7" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="C7" s="49"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:CG3"/>
+  <autoFilter ref="A3:CH3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="15">
-    <mergeCell ref="BL2:BR2"/>
-    <mergeCell ref="BS2:BY2"/>
-    <mergeCell ref="BZ2:CF2"/>
-    <mergeCell ref="AA2:AG2"/>
-    <mergeCell ref="AK2:AM2"/>
-    <mergeCell ref="AN2:AP2"/>
-    <mergeCell ref="AQ2:AW2"/>
-    <mergeCell ref="AX2:BD2"/>
-    <mergeCell ref="BE2:BK2"/>
-    <mergeCell ref="R2:X2"/>
+    <mergeCell ref="S2:Y2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="M2:Q2"/>
     <mergeCell ref="C1:H1"/>
+    <mergeCell ref="BM2:BS2"/>
+    <mergeCell ref="BT2:BZ2"/>
+    <mergeCell ref="CA2:CG2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AO2:AQ2"/>
+    <mergeCell ref="AR2:AX2"/>
+    <mergeCell ref="AY2:BE2"/>
+    <mergeCell ref="BF2:BL2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1845,7 +1861,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Hoja8"/>
   <dimension ref="A2:M11"/>
   <sheetViews>
@@ -1859,58 +1875,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71" t="s">
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71" t="s">
+      <c r="F3" s="61"/>
+      <c r="G3" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="62">
+      <c r="C4" s="63"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="65">
         <v>43685</v>
       </c>
-      <c r="F4" s="63"/>
+      <c r="F4" s="66"/>
       <c r="G4" s="67" t="s">
         <v>6</v>
       </c>
@@ -1925,15 +1941,15 @@
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="62">
+      <c r="C5" s="63"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="65">
         <v>44139</v>
       </c>
-      <c r="F5" s="63"/>
+      <c r="F5" s="66"/>
       <c r="G5" s="67" t="s">
         <v>7</v>
       </c>
@@ -1948,15 +1964,15 @@
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="62" t="s">
+      <c r="C6" s="63"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="63"/>
+      <c r="F6" s="66"/>
       <c r="G6" s="67" t="s">
         <v>10</v>
       </c>
@@ -1971,15 +1987,15 @@
       <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="60"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="62">
+      <c r="C7" s="63"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="65">
         <v>44726</v>
       </c>
-      <c r="F7" s="63"/>
+      <c r="F7" s="66"/>
       <c r="G7" s="67" t="s">
         <v>11</v>
       </c>
@@ -1992,85 +2008,66 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="66"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="72"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="65"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="65"/>
-      <c r="M9" s="66"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="71"/>
+      <c r="M9" s="72"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="66"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71"/>
+      <c r="M10" s="72"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="66"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="71"/>
+      <c r="M11" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:M3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:M5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:M6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:M7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:M8"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:M11"/>
@@ -2080,6 +2077,25 @@
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:M10"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:M7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:M8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:M3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="203" r:id="rId1"/>
@@ -2087,7 +2103,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2098,15 +2114,15 @@
   <sheetData>
     <row r="1" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72" t="s">
+      <c r="C1" s="73"/>
+      <c r="D1" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
       <c r="G1" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
2023-12-05 Se completa modificación de BP.
</commit_message>
<xml_diff>
--- a/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/plantilla_reporte_produccion_historial_cambios_puebla.xlsx
+++ b/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/plantilla_reporte_produccion_historial_cambios_puebla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\NuevoPortal\CódigoFuente\BitacorasProduccion\Content\plantillas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3355BC-40F8-4AB7-B5A6-184B068AEF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3168487C-B3D0-41D1-B705-76308147ACA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Aux" sheetId="5" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$CH$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$CI$3</definedName>
     <definedName name="DATA1" localSheetId="2">#REF!</definedName>
     <definedName name="DATA1" localSheetId="0">#REF!</definedName>
     <definedName name="DATA1">#REF!</definedName>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="83">
   <si>
     <t xml:space="preserve">Control de cambios </t>
   </si>
@@ -351,6 +351,9 @@
   </si>
   <si>
     <t>Cliente</t>
+  </si>
+  <si>
+    <t>¿Posteado?</t>
   </si>
 </sst>
 </file>
@@ -788,7 +791,7 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -935,35 +938,71 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -971,44 +1010,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1300,76 +1306,77 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:CH7"/>
+  <dimension ref="A1:CI7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BR1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R9" sqref="R9"/>
+      <selection pane="bottomLeft" activeCell="CH5" sqref="CH5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="6" customWidth="1"/>
-    <col min="8" max="9" width="11.42578125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="6" customWidth="1"/>
+    <col min="8" max="9" width="11.44140625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" style="6" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" style="6" customWidth="1"/>
     <col min="12" max="13" width="14" style="6" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" style="6" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.28515625" style="6" customWidth="1"/>
-    <col min="18" max="18" width="33.140625" style="6" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="12.44140625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.33203125" style="6" customWidth="1"/>
+    <col min="18" max="18" width="33.109375" style="6" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" style="6" customWidth="1"/>
     <col min="20" max="20" width="19" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.7109375" style="13" customWidth="1"/>
-    <col min="22" max="25" width="12.7109375" style="14" customWidth="1"/>
-    <col min="26" max="27" width="15.28515625" style="15" customWidth="1"/>
-    <col min="28" max="34" width="11.7109375" style="13" customWidth="1"/>
-    <col min="35" max="35" width="13.140625" style="6" customWidth="1"/>
-    <col min="36" max="36" width="10.85546875" style="6" customWidth="1"/>
-    <col min="37" max="37" width="14.140625" style="6" customWidth="1"/>
-    <col min="38" max="38" width="15.140625" style="6" customWidth="1"/>
-    <col min="39" max="39" width="10.42578125" style="6" customWidth="1"/>
-    <col min="40" max="40" width="11.7109375" style="44" customWidth="1"/>
-    <col min="41" max="42" width="11.7109375" style="6" customWidth="1"/>
+    <col min="21" max="21" width="12.6640625" style="13" customWidth="1"/>
+    <col min="22" max="25" width="12.6640625" style="14" customWidth="1"/>
+    <col min="26" max="27" width="15.33203125" style="15" customWidth="1"/>
+    <col min="28" max="34" width="11.6640625" style="13" customWidth="1"/>
+    <col min="35" max="35" width="13.109375" style="6" customWidth="1"/>
+    <col min="36" max="36" width="10.88671875" style="6" customWidth="1"/>
+    <col min="37" max="37" width="14.109375" style="6" customWidth="1"/>
+    <col min="38" max="38" width="15.109375" style="6" customWidth="1"/>
+    <col min="39" max="39" width="10.44140625" style="6" customWidth="1"/>
+    <col min="40" max="40" width="11.6640625" style="44" customWidth="1"/>
+    <col min="41" max="42" width="11.6640625" style="6" customWidth="1"/>
     <col min="43" max="43" width="12" style="6" customWidth="1"/>
-    <col min="44" max="44" width="11.7109375" style="42" customWidth="1"/>
-    <col min="45" max="49" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
-    <col min="50" max="50" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
-    <col min="51" max="56" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
-    <col min="57" max="57" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
-    <col min="58" max="58" width="11.7109375" style="42" customWidth="1"/>
-    <col min="59" max="63" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
-    <col min="64" max="64" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
-    <col min="65" max="70" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
-    <col min="71" max="71" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
-    <col min="72" max="72" width="11.7109375" style="42" customWidth="1"/>
-    <col min="73" max="77" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
-    <col min="78" max="78" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
-    <col min="79" max="84" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
-    <col min="85" max="85" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
-    <col min="86" max="86" width="78.28515625" style="6" customWidth="1"/>
-    <col min="87" max="16384" width="9" style="36"/>
+    <col min="44" max="44" width="11.6640625" style="42" customWidth="1"/>
+    <col min="45" max="49" width="11.6640625" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="50" max="50" width="11.6640625" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="51" max="56" width="11.6640625" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="57" max="57" width="11.6640625" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="58" max="58" width="11.6640625" style="42" customWidth="1"/>
+    <col min="59" max="63" width="11.6640625" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="64" max="64" width="11.6640625" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="65" max="70" width="11.6640625" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="71" max="71" width="11.6640625" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="72" max="72" width="11.6640625" style="42" customWidth="1"/>
+    <col min="73" max="77" width="11.6640625" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="78" max="78" width="11.6640625" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="79" max="84" width="11.6640625" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="85" max="85" width="11.6640625" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="86" max="86" width="10.6640625" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="87" max="87" width="78.33203125" style="6" customWidth="1"/>
+    <col min="88" max="16384" width="9" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:87" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="59" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
       <c r="I1" s="45"/>
       <c r="J1" s="45" t="s">
         <v>15</v>
@@ -1455,125 +1462,127 @@
       <c r="CE1" s="37"/>
       <c r="CF1" s="37"/>
       <c r="CG1" s="43"/>
-      <c r="CH1" s="12"/>
+      <c r="CH1" s="43"/>
+      <c r="CI1" s="12"/>
     </row>
-    <row r="2" spans="1:86" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+    <row r="2" spans="1:87" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="7"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
-      <c r="H2" s="57" t="s">
+      <c r="H2" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="58" t="s">
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
       <c r="R2" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="S2" s="55" t="s">
+      <c r="S2" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="51"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
       <c r="Z2" s="10"/>
       <c r="AA2" s="10"/>
-      <c r="AB2" s="52" t="s">
+      <c r="AB2" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="52"/>
-      <c r="AD2" s="52"/>
-      <c r="AE2" s="52"/>
-      <c r="AF2" s="52"/>
-      <c r="AG2" s="52"/>
-      <c r="AH2" s="52"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="53"/>
+      <c r="AF2" s="53"/>
+      <c r="AG2" s="53"/>
+      <c r="AH2" s="53"/>
       <c r="AI2" s="12"/>
       <c r="AJ2" s="12"/>
       <c r="AK2" s="12"/>
-      <c r="AL2" s="53" t="s">
+      <c r="AL2" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="53" t="s">
+      <c r="AM2" s="59"/>
+      <c r="AN2" s="59"/>
+      <c r="AO2" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="AP2" s="53"/>
-      <c r="AQ2" s="53"/>
-      <c r="AR2" s="54" t="s">
+      <c r="AP2" s="59"/>
+      <c r="AQ2" s="59"/>
+      <c r="AR2" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="54"/>
-      <c r="AW2" s="54"/>
-      <c r="AX2" s="54"/>
-      <c r="AY2" s="54" t="s">
+      <c r="AS2" s="60"/>
+      <c r="AT2" s="60"/>
+      <c r="AU2" s="60"/>
+      <c r="AV2" s="60"/>
+      <c r="AW2" s="60"/>
+      <c r="AX2" s="60"/>
+      <c r="AY2" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="AZ2" s="54"/>
-      <c r="BA2" s="54"/>
-      <c r="BB2" s="54"/>
-      <c r="BC2" s="54"/>
-      <c r="BD2" s="54"/>
-      <c r="BE2" s="54"/>
-      <c r="BF2" s="50" t="s">
+      <c r="AZ2" s="60"/>
+      <c r="BA2" s="60"/>
+      <c r="BB2" s="60"/>
+      <c r="BC2" s="60"/>
+      <c r="BD2" s="60"/>
+      <c r="BE2" s="60"/>
+      <c r="BF2" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="BG2" s="50"/>
-      <c r="BH2" s="50"/>
-      <c r="BI2" s="50"/>
-      <c r="BJ2" s="50"/>
-      <c r="BK2" s="50"/>
-      <c r="BL2" s="50"/>
-      <c r="BM2" s="50" t="s">
+      <c r="BG2" s="57"/>
+      <c r="BH2" s="57"/>
+      <c r="BI2" s="57"/>
+      <c r="BJ2" s="57"/>
+      <c r="BK2" s="57"/>
+      <c r="BL2" s="57"/>
+      <c r="BM2" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="BN2" s="50"/>
-      <c r="BO2" s="50"/>
-      <c r="BP2" s="50"/>
-      <c r="BQ2" s="50"/>
-      <c r="BR2" s="50"/>
-      <c r="BS2" s="50"/>
-      <c r="BT2" s="51" t="s">
+      <c r="BN2" s="57"/>
+      <c r="BO2" s="57"/>
+      <c r="BP2" s="57"/>
+      <c r="BQ2" s="57"/>
+      <c r="BR2" s="57"/>
+      <c r="BS2" s="57"/>
+      <c r="BT2" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="BU2" s="51"/>
-      <c r="BV2" s="51"/>
-      <c r="BW2" s="51"/>
-      <c r="BX2" s="51"/>
-      <c r="BY2" s="51"/>
-      <c r="BZ2" s="51"/>
-      <c r="CA2" s="51" t="s">
+      <c r="BU2" s="58"/>
+      <c r="BV2" s="58"/>
+      <c r="BW2" s="58"/>
+      <c r="BX2" s="58"/>
+      <c r="BY2" s="58"/>
+      <c r="BZ2" s="58"/>
+      <c r="CA2" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="CB2" s="51"/>
-      <c r="CC2" s="51"/>
-      <c r="CD2" s="51"/>
-      <c r="CE2" s="51"/>
-      <c r="CF2" s="51"/>
-      <c r="CG2" s="51"/>
+      <c r="CB2" s="58"/>
+      <c r="CC2" s="58"/>
+      <c r="CD2" s="58"/>
+      <c r="CE2" s="58"/>
+      <c r="CF2" s="58"/>
+      <c r="CG2" s="58"/>
       <c r="CH2" s="12"/>
+      <c r="CI2" s="12"/>
     </row>
-    <row r="3" spans="1:86" s="35" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:87" s="35" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>29</v>
       </c>
@@ -1625,7 +1634,7 @@
       <c r="Q3" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="74" t="s">
+      <c r="R3" s="50" t="s">
         <v>81</v>
       </c>
       <c r="S3" s="20" t="s">
@@ -1829,22 +1838,19 @@
       <c r="CG3" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="CH3" s="34" t="s">
+      <c r="CH3" s="75" t="s">
+        <v>82</v>
+      </c>
+      <c r="CI3" s="34" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:87" x14ac:dyDescent="0.3">
       <c r="C7" s="49"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:CH3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A3:CI3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="15">
-    <mergeCell ref="S2:Y2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="C1:H1"/>
     <mergeCell ref="BM2:BS2"/>
     <mergeCell ref="BT2:BZ2"/>
     <mergeCell ref="CA2:CG2"/>
@@ -1854,6 +1860,12 @@
     <mergeCell ref="AR2:AX2"/>
     <mergeCell ref="AY2:BE2"/>
     <mergeCell ref="BF2:BL2"/>
+    <mergeCell ref="S2:Y2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="C1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1869,205 +1881,224 @@
       <selection activeCell="M23" sqref="M22:M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.3">
+      <c r="A2" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61" t="s">
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61" t="s">
+      <c r="F3" s="73"/>
+      <c r="G3" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="65">
+      <c r="C4" s="62"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="64">
         <v>43685</v>
       </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="67" t="s">
+      <c r="F4" s="65"/>
+      <c r="G4" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="68"/>
-      <c r="M4" s="69"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="71"/>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65">
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="64">
         <v>44139</v>
       </c>
-      <c r="F5" s="66"/>
-      <c r="G5" s="67" t="s">
+      <c r="F5" s="65"/>
+      <c r="G5" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="68"/>
-      <c r="M5" s="69"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="71"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="65" t="s">
+      <c r="C6" s="62"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="66"/>
-      <c r="G6" s="67" t="s">
+      <c r="F6" s="65"/>
+      <c r="G6" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="68"/>
-      <c r="M6" s="69"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="71"/>
     </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="65">
+      <c r="C7" s="62"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="64">
         <v>44726</v>
       </c>
-      <c r="F7" s="66"/>
-      <c r="G7" s="67" t="s">
+      <c r="F7" s="65"/>
+      <c r="G7" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="69"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="71"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="72"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="68"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
-      <c r="B9" s="62"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="72"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="67"/>
+      <c r="M9" s="68"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="70"/>
-      <c r="H10" s="71"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
-      <c r="K10" s="71"/>
-      <c r="L10" s="71"/>
-      <c r="M10" s="72"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="67"/>
+      <c r="M10" s="68"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="71"/>
-      <c r="L11" s="71"/>
-      <c r="M11" s="72"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:M3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:M7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:M8"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:M11"/>
@@ -2077,25 +2108,6 @@
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:M10"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:M7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:M8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:M5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:M6"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:M3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="203" r:id="rId1"/>
@@ -2110,23 +2122,23 @@
       <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73" t="s">
+      <c r="C1" s="74"/>
+      <c r="D1" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>

</xml_diff>

<commit_message>
2025-08-12 BG: Se agrega carga de excel a budget.
</commit_message>
<xml_diff>
--- a/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/plantilla_reporte_produccion_historial_cambios_puebla.xlsx
+++ b/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/plantilla_reporte_produccion_historial_cambios_puebla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\NuevoPortal\CódigoFuente\BitacorasProduccion\Content\plantillas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3168487C-B3D0-41D1-B705-76308147ACA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D6DE80-5610-41D3-8F37-37B74E8B7079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Aux" sheetId="5" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$CI$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$CM$3</definedName>
     <definedName name="DATA1" localSheetId="2">#REF!</definedName>
     <definedName name="DATA1" localSheetId="0">#REF!</definedName>
     <definedName name="DATA1">#REF!</definedName>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="85">
   <si>
     <t xml:space="preserve">Control de cambios </t>
   </si>
@@ -354,6 +354,12 @@
   </si>
   <si>
     <t>¿Posteado?</t>
+  </si>
+  <si>
+    <t>Tipo Metal</t>
+  </si>
+  <si>
+    <t>Molino</t>
   </si>
 </sst>
 </file>
@@ -605,7 +611,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -780,6 +786,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -791,7 +834,7 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -941,35 +984,50 @@
     <xf numFmtId="0" fontId="8" fillId="17" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -987,15 +1045,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1004,16 +1053,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1306,77 +1364,77 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:CI7"/>
+  <dimension ref="A1:CM7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BR1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="CH5" sqref="CH5"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="28.44140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="33.109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="6" customWidth="1"/>
-    <col min="8" max="9" width="11.44140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" style="6" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" style="6" customWidth="1"/>
-    <col min="12" max="13" width="14" style="6" customWidth="1"/>
-    <col min="14" max="14" width="12.44140625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.33203125" style="6" customWidth="1"/>
-    <col min="18" max="18" width="33.109375" style="6" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" style="6" customWidth="1"/>
-    <col min="20" max="20" width="19" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.6640625" style="13" customWidth="1"/>
-    <col min="22" max="25" width="12.6640625" style="14" customWidth="1"/>
-    <col min="26" max="27" width="15.33203125" style="15" customWidth="1"/>
-    <col min="28" max="34" width="11.6640625" style="13" customWidth="1"/>
-    <col min="35" max="35" width="13.109375" style="6" customWidth="1"/>
-    <col min="36" max="36" width="10.88671875" style="6" customWidth="1"/>
-    <col min="37" max="37" width="14.109375" style="6" customWidth="1"/>
-    <col min="38" max="38" width="15.109375" style="6" customWidth="1"/>
-    <col min="39" max="39" width="10.44140625" style="6" customWidth="1"/>
-    <col min="40" max="40" width="11.6640625" style="44" customWidth="1"/>
-    <col min="41" max="42" width="11.6640625" style="6" customWidth="1"/>
-    <col min="43" max="43" width="12" style="6" customWidth="1"/>
-    <col min="44" max="44" width="11.6640625" style="42" customWidth="1"/>
-    <col min="45" max="49" width="11.6640625" style="42" customWidth="1" outlineLevel="1"/>
-    <col min="50" max="50" width="11.6640625" style="44" customWidth="1" outlineLevel="1"/>
-    <col min="51" max="56" width="11.6640625" style="42" customWidth="1" outlineLevel="1"/>
-    <col min="57" max="57" width="11.6640625" style="44" customWidth="1" outlineLevel="1"/>
-    <col min="58" max="58" width="11.6640625" style="42" customWidth="1"/>
-    <col min="59" max="63" width="11.6640625" style="42" customWidth="1" outlineLevel="1"/>
-    <col min="64" max="64" width="11.6640625" style="44" customWidth="1" outlineLevel="1"/>
-    <col min="65" max="70" width="11.6640625" style="42" customWidth="1" outlineLevel="1"/>
-    <col min="71" max="71" width="11.6640625" style="44" customWidth="1" outlineLevel="1"/>
-    <col min="72" max="72" width="11.6640625" style="42" customWidth="1"/>
-    <col min="73" max="77" width="11.6640625" style="42" customWidth="1" outlineLevel="1"/>
-    <col min="78" max="78" width="11.6640625" style="44" customWidth="1" outlineLevel="1"/>
-    <col min="79" max="84" width="11.6640625" style="42" customWidth="1" outlineLevel="1"/>
-    <col min="85" max="85" width="11.6640625" style="44" customWidth="1" outlineLevel="1"/>
-    <col min="86" max="86" width="10.6640625" style="44" customWidth="1" outlineLevel="1"/>
-    <col min="87" max="87" width="78.33203125" style="6" customWidth="1"/>
-    <col min="88" max="16384" width="9" style="36"/>
+    <col min="1" max="1" width="10.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="6" customWidth="1"/>
+    <col min="8" max="9" width="11.42578125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="6" customWidth="1"/>
+    <col min="12" max="15" width="14" style="6" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" style="6" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="12.28515625" style="6" customWidth="1"/>
+    <col min="22" max="22" width="33.140625" style="6" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" style="6" customWidth="1"/>
+    <col min="24" max="24" width="19" style="6" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="13" customWidth="1"/>
+    <col min="26" max="29" width="12.7109375" style="14" customWidth="1"/>
+    <col min="30" max="31" width="15.28515625" style="15" customWidth="1"/>
+    <col min="32" max="38" width="11.7109375" style="13" customWidth="1"/>
+    <col min="39" max="39" width="13.140625" style="6" customWidth="1"/>
+    <col min="40" max="40" width="10.85546875" style="6" customWidth="1"/>
+    <col min="41" max="41" width="14.140625" style="6" customWidth="1"/>
+    <col min="42" max="42" width="15.140625" style="6" customWidth="1"/>
+    <col min="43" max="43" width="10.42578125" style="6" customWidth="1"/>
+    <col min="44" max="44" width="11.7109375" style="44" customWidth="1"/>
+    <col min="45" max="46" width="11.7109375" style="6" customWidth="1"/>
+    <col min="47" max="47" width="12" style="6" customWidth="1"/>
+    <col min="48" max="48" width="11.7109375" style="42" customWidth="1"/>
+    <col min="49" max="53" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="54" max="54" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="55" max="60" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="61" max="61" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="11.7109375" style="42" customWidth="1"/>
+    <col min="63" max="67" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="69" max="74" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="75" max="75" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="76" max="76" width="11.7109375" style="42" customWidth="1"/>
+    <col min="77" max="81" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="82" max="82" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="83" max="88" width="11.7109375" style="42" customWidth="1" outlineLevel="1"/>
+    <col min="89" max="89" width="11.7109375" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="90" max="90" width="10.7109375" style="44" customWidth="1" outlineLevel="1"/>
+    <col min="91" max="91" width="78.28515625" style="6" customWidth="1"/>
+    <col min="92" max="16384" width="9" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:91" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="56" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
       <c r="I1" s="45"/>
       <c r="J1" s="45" t="s">
         <v>15</v>
@@ -1385,23 +1443,23 @@
       <c r="L1" s="45"/>
       <c r="M1" s="45"/>
       <c r="N1" s="45"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
       <c r="S1" s="12"/>
       <c r="T1" s="12"/>
       <c r="U1" s="12"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
       <c r="AF1" s="12"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
@@ -1410,179 +1468,187 @@
       <c r="AK1" s="12"/>
       <c r="AL1" s="12"/>
       <c r="AM1" s="12"/>
-      <c r="AN1" s="43"/>
+      <c r="AN1" s="12"/>
       <c r="AO1" s="12"/>
       <c r="AP1" s="12"/>
       <c r="AQ1" s="12"/>
-      <c r="AR1" s="37" t="s">
+      <c r="AR1" s="43"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="AS1" s="37"/>
-      <c r="AT1" s="37"/>
-      <c r="AU1" s="37"/>
-      <c r="AV1" s="37"/>
       <c r="AW1" s="37"/>
-      <c r="AX1" s="43"/>
+      <c r="AX1" s="37"/>
       <c r="AY1" s="37"/>
       <c r="AZ1" s="37"/>
       <c r="BA1" s="37"/>
-      <c r="BB1" s="37"/>
+      <c r="BB1" s="43"/>
       <c r="BC1" s="37"/>
       <c r="BD1" s="37"/>
-      <c r="BE1" s="43"/>
-      <c r="BF1" s="37" t="s">
-        <v>17</v>
-      </c>
+      <c r="BE1" s="37"/>
+      <c r="BF1" s="37"/>
       <c r="BG1" s="37"/>
       <c r="BH1" s="37"/>
-      <c r="BI1" s="37"/>
-      <c r="BJ1" s="37"/>
+      <c r="BI1" s="43"/>
+      <c r="BJ1" s="37" t="s">
+        <v>17</v>
+      </c>
       <c r="BK1" s="37"/>
-      <c r="BL1" s="43"/>
+      <c r="BL1" s="37"/>
       <c r="BM1" s="37"/>
       <c r="BN1" s="37"/>
       <c r="BO1" s="37"/>
-      <c r="BP1" s="37"/>
+      <c r="BP1" s="43"/>
       <c r="BQ1" s="37"/>
       <c r="BR1" s="37"/>
-      <c r="BS1" s="43"/>
-      <c r="BT1" s="37" t="s">
-        <v>80</v>
-      </c>
+      <c r="BS1" s="37"/>
+      <c r="BT1" s="37"/>
       <c r="BU1" s="37"/>
       <c r="BV1" s="37"/>
-      <c r="BW1" s="37"/>
-      <c r="BX1" s="37"/>
+      <c r="BW1" s="43"/>
+      <c r="BX1" s="37" t="s">
+        <v>80</v>
+      </c>
       <c r="BY1" s="37"/>
-      <c r="BZ1" s="43"/>
+      <c r="BZ1" s="37"/>
       <c r="CA1" s="37"/>
       <c r="CB1" s="37"/>
       <c r="CC1" s="37"/>
-      <c r="CD1" s="37"/>
+      <c r="CD1" s="43"/>
       <c r="CE1" s="37"/>
       <c r="CF1" s="37"/>
-      <c r="CG1" s="43"/>
-      <c r="CH1" s="43"/>
-      <c r="CI1" s="12"/>
+      <c r="CG1" s="37"/>
+      <c r="CH1" s="37"/>
+      <c r="CI1" s="37"/>
+      <c r="CJ1" s="37"/>
+      <c r="CK1" s="43"/>
+      <c r="CL1" s="43"/>
+      <c r="CM1" s="12"/>
     </row>
-    <row r="2" spans="1:87" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:91" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
       <c r="E2" s="7"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="55" t="s">
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="48" t="s">
+      <c r="P2" s="79"/>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="79"/>
+      <c r="U2" s="80"/>
+      <c r="V2" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="S2" s="51" t="s">
+      <c r="W2" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="53" t="s">
+      <c r="X2" s="58"/>
+      <c r="Y2" s="58"/>
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="58"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="58"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
-      <c r="AF2" s="53"/>
-      <c r="AG2" s="53"/>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="12"/>
-      <c r="AJ2" s="12"/>
-      <c r="AK2" s="12"/>
-      <c r="AL2" s="59" t="s">
+      <c r="AG2" s="55"/>
+      <c r="AH2" s="55"/>
+      <c r="AI2" s="55"/>
+      <c r="AJ2" s="55"/>
+      <c r="AK2" s="55"/>
+      <c r="AL2" s="55"/>
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="12"/>
+      <c r="AO2" s="12"/>
+      <c r="AP2" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="AM2" s="59"/>
-      <c r="AN2" s="59"/>
-      <c r="AO2" s="59" t="s">
+      <c r="AQ2" s="56"/>
+      <c r="AR2" s="56"/>
+      <c r="AS2" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="AP2" s="59"/>
-      <c r="AQ2" s="59"/>
-      <c r="AR2" s="60" t="s">
+      <c r="AT2" s="56"/>
+      <c r="AU2" s="56"/>
+      <c r="AV2" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="AS2" s="60"/>
-      <c r="AT2" s="60"/>
-      <c r="AU2" s="60"/>
-      <c r="AV2" s="60"/>
-      <c r="AW2" s="60"/>
-      <c r="AX2" s="60"/>
-      <c r="AY2" s="60" t="s">
+      <c r="AW2" s="57"/>
+      <c r="AX2" s="57"/>
+      <c r="AY2" s="57"/>
+      <c r="AZ2" s="57"/>
+      <c r="BA2" s="57"/>
+      <c r="BB2" s="57"/>
+      <c r="BC2" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="AZ2" s="60"/>
-      <c r="BA2" s="60"/>
-      <c r="BB2" s="60"/>
-      <c r="BC2" s="60"/>
-      <c r="BD2" s="60"/>
-      <c r="BE2" s="60"/>
-      <c r="BF2" s="57" t="s">
-        <v>25</v>
-      </c>
+      <c r="BD2" s="57"/>
+      <c r="BE2" s="57"/>
+      <c r="BF2" s="57"/>
       <c r="BG2" s="57"/>
       <c r="BH2" s="57"/>
       <c r="BI2" s="57"/>
-      <c r="BJ2" s="57"/>
-      <c r="BK2" s="57"/>
-      <c r="BL2" s="57"/>
-      <c r="BM2" s="57" t="s">
+      <c r="BJ2" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="BK2" s="53"/>
+      <c r="BL2" s="53"/>
+      <c r="BM2" s="53"/>
+      <c r="BN2" s="53"/>
+      <c r="BO2" s="53"/>
+      <c r="BP2" s="53"/>
+      <c r="BQ2" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="BN2" s="57"/>
-      <c r="BO2" s="57"/>
-      <c r="BP2" s="57"/>
-      <c r="BQ2" s="57"/>
-      <c r="BR2" s="57"/>
-      <c r="BS2" s="57"/>
-      <c r="BT2" s="58" t="s">
+      <c r="BR2" s="53"/>
+      <c r="BS2" s="53"/>
+      <c r="BT2" s="53"/>
+      <c r="BU2" s="53"/>
+      <c r="BV2" s="53"/>
+      <c r="BW2" s="53"/>
+      <c r="BX2" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="BU2" s="58"/>
-      <c r="BV2" s="58"/>
-      <c r="BW2" s="58"/>
-      <c r="BX2" s="58"/>
-      <c r="BY2" s="58"/>
-      <c r="BZ2" s="58"/>
-      <c r="CA2" s="58" t="s">
+      <c r="BY2" s="54"/>
+      <c r="BZ2" s="54"/>
+      <c r="CA2" s="54"/>
+      <c r="CB2" s="54"/>
+      <c r="CC2" s="54"/>
+      <c r="CD2" s="54"/>
+      <c r="CE2" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="CB2" s="58"/>
-      <c r="CC2" s="58"/>
-      <c r="CD2" s="58"/>
-      <c r="CE2" s="58"/>
-      <c r="CF2" s="58"/>
-      <c r="CG2" s="58"/>
-      <c r="CH2" s="12"/>
-      <c r="CI2" s="12"/>
+      <c r="CF2" s="54"/>
+      <c r="CG2" s="54"/>
+      <c r="CH2" s="54"/>
+      <c r="CI2" s="54"/>
+      <c r="CJ2" s="54"/>
+      <c r="CK2" s="54"/>
+      <c r="CL2" s="12"/>
+      <c r="CM2" s="12"/>
     </row>
-    <row r="3" spans="1:87" s="35" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:91" s="35" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>29</v>
       </c>
@@ -1619,253 +1685,265 @@
       <c r="L3" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="M3" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="O3" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="P3" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="Q3" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="P3" s="19" t="s">
+      <c r="R3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="19" t="s">
+      <c r="S3" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="50" t="s">
+      <c r="T3" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="U3" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="V3" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="S3" s="20" t="s">
+      <c r="W3" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="T3" s="20" t="s">
+      <c r="X3" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="U3" s="20" t="s">
+      <c r="Y3" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="V3" s="21" t="s">
+      <c r="Z3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="W3" s="21" t="s">
+      <c r="AA3" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="X3" s="21" t="s">
+      <c r="AB3" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="Y3" s="21" t="s">
+      <c r="AC3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="Z3" s="22" t="s">
+      <c r="AD3" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="AA3" s="23" t="s">
+      <c r="AE3" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="AB3" s="24" t="s">
+      <c r="AF3" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="AC3" s="25" t="s">
+      <c r="AG3" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="AD3" s="25" t="s">
+      <c r="AH3" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="AE3" s="25" t="s">
+      <c r="AI3" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="AF3" s="26" t="s">
+      <c r="AJ3" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AG3" s="26" t="s">
+      <c r="AK3" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="AH3" s="27" t="s">
+      <c r="AL3" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="AI3" s="16" t="s">
+      <c r="AM3" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="AJ3" s="16" t="s">
+      <c r="AN3" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="AK3" s="16" t="s">
+      <c r="AO3" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="AL3" s="16" t="s">
+      <c r="AP3" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="AM3" s="16" t="s">
+      <c r="AQ3" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="AN3" s="28" t="s">
+      <c r="AR3" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="AO3" s="29" t="s">
+      <c r="AS3" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="AP3" s="29" t="s">
+      <c r="AT3" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="AQ3" s="16" t="s">
+      <c r="AU3" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="AR3" s="38" t="s">
+      <c r="AV3" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="AS3" s="38" t="s">
+      <c r="AW3" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="AT3" s="38" t="s">
+      <c r="AX3" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="AU3" s="38" t="s">
+      <c r="AY3" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="AV3" s="38" t="s">
+      <c r="AZ3" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="AW3" s="38" t="s">
+      <c r="BA3" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="AX3" s="30" t="s">
+      <c r="BB3" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="AY3" s="39" t="s">
+      <c r="BC3" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="AZ3" s="39" t="s">
+      <c r="BD3" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="BA3" s="39" t="s">
+      <c r="BE3" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="BB3" s="46" t="s">
+      <c r="BF3" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="BC3" s="39" t="s">
+      <c r="BG3" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="BD3" s="39" t="s">
+      <c r="BH3" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="BE3" s="31" t="s">
+      <c r="BI3" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="BF3" s="40" t="s">
+      <c r="BJ3" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="BG3" s="40" t="s">
+      <c r="BK3" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="BH3" s="40" t="s">
+      <c r="BL3" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="BI3" s="40" t="s">
+      <c r="BM3" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="BJ3" s="40" t="s">
+      <c r="BN3" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="BK3" s="40" t="s">
+      <c r="BO3" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="BL3" s="32" t="s">
+      <c r="BP3" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="BM3" s="41" t="s">
+      <c r="BQ3" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="BN3" s="41" t="s">
+      <c r="BR3" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="BO3" s="41" t="s">
+      <c r="BS3" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="BP3" s="47" t="s">
+      <c r="BT3" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="BQ3" s="41" t="s">
+      <c r="BU3" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="BR3" s="41" t="s">
+      <c r="BV3" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="BS3" s="33" t="s">
+      <c r="BW3" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="BT3" s="40" t="s">
+      <c r="BX3" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="BU3" s="40" t="s">
+      <c r="BY3" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="BV3" s="40" t="s">
+      <c r="BZ3" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="BW3" s="40" t="s">
+      <c r="CA3" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="BX3" s="40" t="s">
+      <c r="CB3" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="BY3" s="40" t="s">
+      <c r="CC3" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="BZ3" s="32" t="s">
+      <c r="CD3" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="CA3" s="41" t="s">
+      <c r="CE3" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="CB3" s="41" t="s">
+      <c r="CF3" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="CC3" s="41" t="s">
+      <c r="CG3" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="CD3" s="47" t="s">
+      <c r="CH3" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="CE3" s="41" t="s">
+      <c r="CI3" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="CF3" s="41" t="s">
+      <c r="CJ3" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="CG3" s="33" t="s">
+      <c r="CK3" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="CH3" s="75" t="s">
+      <c r="CL3" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="CI3" s="34" t="s">
+      <c r="CM3" s="34" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:87" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:91" x14ac:dyDescent="0.25">
       <c r="C7" s="49"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:CI3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A3:CM3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="15">
-    <mergeCell ref="BM2:BS2"/>
-    <mergeCell ref="BT2:BZ2"/>
-    <mergeCell ref="CA2:CG2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="AO2:AQ2"/>
-    <mergeCell ref="AR2:AX2"/>
-    <mergeCell ref="AY2:BE2"/>
-    <mergeCell ref="BF2:BL2"/>
-    <mergeCell ref="S2:Y2"/>
+    <mergeCell ref="W2:AC2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="M2:Q2"/>
     <mergeCell ref="C1:H1"/>
+    <mergeCell ref="O2:U2"/>
+    <mergeCell ref="H2:N2"/>
+    <mergeCell ref="BQ2:BW2"/>
+    <mergeCell ref="BX2:CD2"/>
+    <mergeCell ref="CE2:CK2"/>
+    <mergeCell ref="AF2:AL2"/>
+    <mergeCell ref="AP2:AR2"/>
+    <mergeCell ref="AS2:AU2"/>
+    <mergeCell ref="AV2:BB2"/>
+    <mergeCell ref="BC2:BI2"/>
+    <mergeCell ref="BJ2:BP2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1881,224 +1959,205 @@
       <selection activeCell="M23" sqref="M22:M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="11.44140625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.3">
-      <c r="A2" s="72" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73" t="s">
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73" t="s">
+      <c r="F3" s="65"/>
+      <c r="G3" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="64">
+      <c r="C4" s="67"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="69">
         <v>43685</v>
       </c>
-      <c r="F4" s="65"/>
-      <c r="G4" s="69" t="s">
+      <c r="F4" s="70"/>
+      <c r="G4" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="71"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="73"/>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="64">
+      <c r="C5" s="67"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="69">
         <v>44139</v>
       </c>
-      <c r="F5" s="65"/>
-      <c r="G5" s="69" t="s">
+      <c r="F5" s="70"/>
+      <c r="G5" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="71"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="73"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="64" t="s">
+      <c r="C6" s="67"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="69" t="s">
+      <c r="F6" s="70"/>
+      <c r="G6" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="71"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="73"/>
     </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="64">
+      <c r="C7" s="67"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="69">
         <v>44726</v>
       </c>
-      <c r="F7" s="65"/>
-      <c r="G7" s="69" t="s">
+      <c r="F7" s="70"/>
+      <c r="G7" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="70"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="70"/>
-      <c r="K7" s="70"/>
-      <c r="L7" s="70"/>
-      <c r="M7" s="71"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="73"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="68"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="75"/>
+      <c r="M8" s="76"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="68"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="76"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="68"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="75"/>
+      <c r="M10" s="76"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="68"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="75"/>
+      <c r="L11" s="75"/>
+      <c r="M11" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:M3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:M5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:M6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:M7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:M8"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:M11"/>
@@ -2108,6 +2167,25 @@
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:M10"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:M7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:M8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:M3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="203" r:id="rId1"/>
@@ -2122,23 +2200,23 @@
       <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74" t="s">
+      <c r="C1" s="77"/>
+      <c r="D1" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>

</xml_diff>

<commit_message>
2025-08-20 SCDM:Se añade signal a herramienta MD.
</commit_message>
<xml_diff>
--- a/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/plantilla_reporte_produccion_historial_cambios_puebla.xlsx
+++ b/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/plantilla_reporte_produccion_historial_cambios_puebla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\NuevoPortal\CódigoFuente\BitacorasProduccion\Content\plantillas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D6DE80-5610-41D3-8F37-37B74E8B7079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224227B3-F1E6-4D0F-ABA2-E6F0D4A2C30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -356,10 +356,10 @@
     <t>¿Posteado?</t>
   </si>
   <si>
-    <t>Tipo Metal</t>
-  </si>
-  <si>
     <t>Molino</t>
+  </si>
+  <si>
+    <t>Superficie</t>
   </si>
 </sst>
 </file>
@@ -990,89 +990,89 @@
     <xf numFmtId="0" fontId="8" fillId="18" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1368,7 +1368,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2:N2"/>
+      <selection pane="bottomLeft" activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1423,18 +1423,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:91" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
       <c r="I1" s="45"/>
       <c r="J1" s="45" t="s">
         <v>15</v>
@@ -1546,27 +1546,27 @@
       <c r="L2" s="61"/>
       <c r="M2" s="61"/>
       <c r="N2" s="62"/>
-      <c r="O2" s="78" t="s">
+      <c r="O2" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="80"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="59"/>
       <c r="V2" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="W2" s="58" t="s">
+      <c r="W2" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="X2" s="58"/>
-      <c r="Y2" s="58"/>
-      <c r="Z2" s="58"/>
-      <c r="AA2" s="58"/>
-      <c r="AB2" s="58"/>
-      <c r="AC2" s="58"/>
+      <c r="X2" s="53"/>
+      <c r="Y2" s="53"/>
+      <c r="Z2" s="53"/>
+      <c r="AA2" s="53"/>
+      <c r="AB2" s="53"/>
+      <c r="AC2" s="53"/>
       <c r="AD2" s="10"/>
       <c r="AE2" s="10"/>
       <c r="AF2" s="55" t="s">
@@ -1581,70 +1581,70 @@
       <c r="AM2" s="12"/>
       <c r="AN2" s="12"/>
       <c r="AO2" s="12"/>
-      <c r="AP2" s="56" t="s">
+      <c r="AP2" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="AQ2" s="56"/>
-      <c r="AR2" s="56"/>
-      <c r="AS2" s="56" t="s">
+      <c r="AQ2" s="65"/>
+      <c r="AR2" s="65"/>
+      <c r="AS2" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="AT2" s="56"/>
-      <c r="AU2" s="56"/>
-      <c r="AV2" s="57" t="s">
+      <c r="AT2" s="65"/>
+      <c r="AU2" s="65"/>
+      <c r="AV2" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="AW2" s="57"/>
-      <c r="AX2" s="57"/>
-      <c r="AY2" s="57"/>
-      <c r="AZ2" s="57"/>
-      <c r="BA2" s="57"/>
-      <c r="BB2" s="57"/>
-      <c r="BC2" s="57" t="s">
+      <c r="AW2" s="66"/>
+      <c r="AX2" s="66"/>
+      <c r="AY2" s="66"/>
+      <c r="AZ2" s="66"/>
+      <c r="BA2" s="66"/>
+      <c r="BB2" s="66"/>
+      <c r="BC2" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="BD2" s="57"/>
-      <c r="BE2" s="57"/>
-      <c r="BF2" s="57"/>
-      <c r="BG2" s="57"/>
-      <c r="BH2" s="57"/>
-      <c r="BI2" s="57"/>
-      <c r="BJ2" s="53" t="s">
+      <c r="BD2" s="66"/>
+      <c r="BE2" s="66"/>
+      <c r="BF2" s="66"/>
+      <c r="BG2" s="66"/>
+      <c r="BH2" s="66"/>
+      <c r="BI2" s="66"/>
+      <c r="BJ2" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="BK2" s="53"/>
-      <c r="BL2" s="53"/>
-      <c r="BM2" s="53"/>
-      <c r="BN2" s="53"/>
-      <c r="BO2" s="53"/>
-      <c r="BP2" s="53"/>
-      <c r="BQ2" s="53" t="s">
+      <c r="BK2" s="63"/>
+      <c r="BL2" s="63"/>
+      <c r="BM2" s="63"/>
+      <c r="BN2" s="63"/>
+      <c r="BO2" s="63"/>
+      <c r="BP2" s="63"/>
+      <c r="BQ2" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="BR2" s="53"/>
-      <c r="BS2" s="53"/>
-      <c r="BT2" s="53"/>
-      <c r="BU2" s="53"/>
-      <c r="BV2" s="53"/>
-      <c r="BW2" s="53"/>
-      <c r="BX2" s="54" t="s">
+      <c r="BR2" s="63"/>
+      <c r="BS2" s="63"/>
+      <c r="BT2" s="63"/>
+      <c r="BU2" s="63"/>
+      <c r="BV2" s="63"/>
+      <c r="BW2" s="63"/>
+      <c r="BX2" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="BY2" s="54"/>
-      <c r="BZ2" s="54"/>
-      <c r="CA2" s="54"/>
-      <c r="CB2" s="54"/>
-      <c r="CC2" s="54"/>
-      <c r="CD2" s="54"/>
-      <c r="CE2" s="54" t="s">
+      <c r="BY2" s="64"/>
+      <c r="BZ2" s="64"/>
+      <c r="CA2" s="64"/>
+      <c r="CB2" s="64"/>
+      <c r="CC2" s="64"/>
+      <c r="CD2" s="64"/>
+      <c r="CE2" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="CF2" s="54"/>
-      <c r="CG2" s="54"/>
-      <c r="CH2" s="54"/>
-      <c r="CI2" s="54"/>
-      <c r="CJ2" s="54"/>
-      <c r="CK2" s="54"/>
+      <c r="CF2" s="64"/>
+      <c r="CG2" s="64"/>
+      <c r="CH2" s="64"/>
+      <c r="CI2" s="64"/>
+      <c r="CJ2" s="64"/>
+      <c r="CK2" s="64"/>
       <c r="CL2" s="12"/>
       <c r="CM2" s="12"/>
     </row>
@@ -1686,10 +1686,10 @@
         <v>39</v>
       </c>
       <c r="M3" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="N3" s="18" t="s">
         <v>83</v>
-      </c>
-      <c r="N3" s="18" t="s">
-        <v>84</v>
       </c>
       <c r="O3" s="19" t="s">
         <v>40</v>
@@ -1707,10 +1707,10 @@
         <v>39</v>
       </c>
       <c r="T3" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="U3" s="52" t="s">
         <v>83</v>
-      </c>
-      <c r="U3" s="52" t="s">
-        <v>84</v>
       </c>
       <c r="V3" s="50" t="s">
         <v>81</v>
@@ -1929,12 +1929,6 @@
   </sheetData>
   <autoFilter ref="A3:CM3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="15">
-    <mergeCell ref="W2:AC2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="O2:U2"/>
-    <mergeCell ref="H2:N2"/>
     <mergeCell ref="BQ2:BW2"/>
     <mergeCell ref="BX2:CD2"/>
     <mergeCell ref="CE2:CK2"/>
@@ -1944,6 +1938,12 @@
     <mergeCell ref="AV2:BB2"/>
     <mergeCell ref="BC2:BI2"/>
     <mergeCell ref="BJ2:BP2"/>
+    <mergeCell ref="W2:AC2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="O2:U2"/>
+    <mergeCell ref="H2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1965,199 +1965,218 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65" t="s">
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65" t="s">
+      <c r="F3" s="79"/>
+      <c r="G3" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="69">
+      <c r="C4" s="68"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="70">
         <v>43685</v>
       </c>
-      <c r="F4" s="70"/>
-      <c r="G4" s="71" t="s">
+      <c r="F4" s="71"/>
+      <c r="G4" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="73"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="77"/>
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="69">
+      <c r="C5" s="68"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="70">
         <v>44139</v>
       </c>
-      <c r="F5" s="70"/>
-      <c r="G5" s="71" t="s">
+      <c r="F5" s="71"/>
+      <c r="G5" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="73"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="77"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="69" t="s">
+      <c r="C6" s="68"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="70"/>
-      <c r="G6" s="71" t="s">
+      <c r="F6" s="71"/>
+      <c r="G6" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="73"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="77"/>
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="69">
+      <c r="C7" s="68"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="70">
         <v>44726</v>
       </c>
-      <c r="F7" s="70"/>
-      <c r="G7" s="71" t="s">
+      <c r="F7" s="71"/>
+      <c r="G7" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="73"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="77"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="76"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="74"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="76"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="74"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="76"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="74"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="66"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="76"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:M3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:M7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:M8"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:M11"/>
@@ -2167,25 +2186,6 @@
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:M10"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:M7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:M8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:M5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:M6"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:M3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="203" r:id="rId1"/>
@@ -2204,15 +2204,15 @@
   <sheetData>
     <row r="1" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77" t="s">
+      <c r="C1" s="80"/>
+      <c r="D1" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
       <c r="G1" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>